<commit_message>
Cast C03 and created C04 template
</commit_message>
<xml_diff>
--- a/Charge 13 - C03.xlsx
+++ b/Charge 13 - C03.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Elements Data" sheetId="4" r:id="rId1"/>
     <sheet name="Lab Print" sheetId="19" r:id="rId2"/>
-    <sheet name="Charge 12" sheetId="13" r:id="rId3"/>
+    <sheet name="Charge 13" sheetId="13" r:id="rId3"/>
     <sheet name="A" sheetId="14" r:id="rId4"/>
     <sheet name="B" sheetId="15" r:id="rId5"/>
     <sheet name="C" sheetId="16" r:id="rId6"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">A!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">B!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'C'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Charge 12'!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Charge 13'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">D!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">E!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Elements Data'!$A$1:$K$48</definedName>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="198">
   <si>
     <t>Mg</t>
   </si>
@@ -832,6 +832,18 @@
   </si>
   <si>
     <t>Charge 13 - C03</t>
+  </si>
+  <si>
+    <t>Held at 510 for 30 seconds</t>
+  </si>
+  <si>
+    <t>Then stirred melt before casting</t>
+  </si>
+  <si>
+    <t>Stirred melt at high temp of each heating cycle</t>
+  </si>
+  <si>
+    <t>Held melt at 510C for 30 seconds and stirred just before casting</t>
   </si>
 </sst>
 </file>
@@ -4874,7 +4886,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="170" t="str">
-        <f>'Charge 12'!A1:G1</f>
+        <f>'Charge 13'!A1:G1</f>
         <v>Charge 13 - C03</v>
       </c>
       <c r="B1" s="171"/>
@@ -4886,7 +4898,7 @@
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="173" t="str">
-        <f>"Nominal  " &amp; 'Charge 12'!A3</f>
+        <f>"Nominal  " &amp; 'Charge 13'!A3</f>
         <v>Nominal  Mg65Zn30Ca5</v>
       </c>
       <c r="B2" s="174"/>
@@ -4898,8 +4910,8 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="173" t="str">
-        <f>"Actual  " &amp; 'Charge 12'!I3</f>
-        <v>Actual  Mg0Ca100</v>
+        <f>"Actual  " &amp; 'Charge 13'!I3</f>
+        <v>Actual  Mg65Zn30Ca5</v>
       </c>
       <c r="B3" s="174"/>
       <c r="C3" s="174"/>
@@ -4913,23 +4925,23 @@
         <v>170</v>
       </c>
       <c r="B4" s="134" t="str">
-        <f>'Charge 12'!Q4</f>
+        <f>'Charge 13'!Q4</f>
         <v>Mg</v>
       </c>
       <c r="C4" s="132" t="str">
-        <f>'Charge 12'!Q5</f>
+        <f>'Charge 13'!Q5</f>
         <v>Zn</v>
       </c>
       <c r="D4" s="133" t="str">
-        <f>'Charge 12'!Q6</f>
+        <f>'Charge 13'!Q6</f>
         <v>Ca</v>
       </c>
       <c r="E4" s="154" t="str">
-        <f>'Charge 12'!Q7</f>
+        <f>'Charge 13'!Q7</f>
         <v>D</v>
       </c>
       <c r="F4" s="152" t="str">
-        <f>'Charge 12'!Q8</f>
+        <f>'Charge 13'!Q8</f>
         <v>E</v>
       </c>
       <c r="G4" s="149" t="s">
@@ -4961,29 +4973,29 @@
       <c r="A6" s="26">
         <v>1</v>
       </c>
-      <c r="B6" s="105" t="str">
-        <f>IF('Charge 12'!B14=0, "-", 'Charge 12'!B14)</f>
+      <c r="B6" s="105">
+        <f>IF('Charge 13'!B14=0, "-", 'Charge 13'!B14)</f>
+        <v>5.0609999999999999</v>
+      </c>
+      <c r="C6" s="137">
+        <f>IF('Charge 13'!E14=0,"-",'Charge 13'!E14)</f>
+        <v>10.72</v>
+      </c>
+      <c r="D6" s="137">
+        <f>IF('Charge 13'!H14=0, "-", 'Charge 13'!H14)</f>
+        <v>3.052</v>
+      </c>
+      <c r="E6" s="137" t="str">
+        <f>IF('Charge 13'!K14=0, "-", 'Charge 13'!K14)</f>
         <v>-</v>
       </c>
-      <c r="C6" s="137" t="str">
-        <f>IF('Charge 12'!E14=0,"-",'Charge 12'!E14)</f>
-        <v>-</v>
-      </c>
-      <c r="D6" s="137">
-        <f>IF('Charge 12'!H14=0, "-", 'Charge 12'!H14)</f>
-        <v>6.101</v>
-      </c>
-      <c r="E6" s="137" t="str">
-        <f>IF('Charge 12'!K14=0, "-", 'Charge 12'!K14)</f>
-        <v>-</v>
-      </c>
       <c r="F6" s="138" t="str">
-        <f>IF('Charge 12'!N14=0, "-", 'Charge 12'!N14)</f>
+        <f>IF('Charge 13'!N14=0, "-", 'Charge 13'!N14)</f>
         <v>-</v>
       </c>
       <c r="G6" s="138">
         <f>COUNTIF(B6:B20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="131" t="str">
         <f>B4</f>
@@ -4994,29 +5006,29 @@
       <c r="A7" s="27">
         <v>2</v>
       </c>
-      <c r="B7" s="108" t="str">
-        <f>IF('Charge 12'!B15=0, "-", 'Charge 12'!B15)</f>
+      <c r="B7" s="108">
+        <f>IF('Charge 13'!B15=0, "-", 'Charge 13'!B15)</f>
+        <v>5.6879999999999997</v>
+      </c>
+      <c r="C7" s="107">
+        <f>IF('Charge 13'!E15=0,"-",'Charge 13'!E15)</f>
+        <v>19.149000000000001</v>
+      </c>
+      <c r="D7" s="107" t="str">
+        <f>IF('Charge 13'!H15=0, "-", 'Charge 13'!H15)</f>
         <v>-</v>
       </c>
-      <c r="C7" s="107" t="str">
-        <f>IF('Charge 12'!E15=0,"-",'Charge 12'!E15)</f>
+      <c r="E7" s="107" t="str">
+        <f>IF('Charge 13'!K15=0, "-", 'Charge 13'!K15)</f>
         <v>-</v>
       </c>
-      <c r="D7" s="107" t="str">
-        <f>IF('Charge 12'!H15=0, "-", 'Charge 12'!H15)</f>
-        <v>-</v>
-      </c>
-      <c r="E7" s="107" t="str">
-        <f>IF('Charge 12'!K15=0, "-", 'Charge 12'!K15)</f>
-        <v>-</v>
-      </c>
       <c r="F7" s="106" t="str">
-        <f>IF('Charge 12'!N15=0, "-", 'Charge 12'!N15)</f>
+        <f>IF('Charge 13'!N15=0, "-", 'Charge 13'!N15)</f>
         <v>-</v>
       </c>
       <c r="G7" s="106">
         <f>COUNTIF(C6:C20, "&lt;&gt;-")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="151" t="str">
         <f>C4</f>
@@ -5027,24 +5039,24 @@
       <c r="A8" s="27">
         <v>3</v>
       </c>
-      <c r="B8" s="108" t="str">
-        <f>IF('Charge 12'!B16=0, "-", 'Charge 12'!B16)</f>
+      <c r="B8" s="108">
+        <f>IF('Charge 13'!B16=0, "-", 'Charge 13'!B16)</f>
+        <v>6.0830000000000002</v>
+      </c>
+      <c r="C8" s="107" t="str">
+        <f>IF('Charge 13'!E16=0,"-",'Charge 13'!E16)</f>
         <v>-</v>
       </c>
-      <c r="C8" s="107" t="str">
-        <f>IF('Charge 12'!E16=0,"-",'Charge 12'!E16)</f>
+      <c r="D8" s="107" t="str">
+        <f>IF('Charge 13'!H16=0, "-", 'Charge 13'!H16)</f>
         <v>-</v>
       </c>
-      <c r="D8" s="107" t="str">
-        <f>IF('Charge 12'!H16=0, "-", 'Charge 12'!H16)</f>
+      <c r="E8" s="107" t="str">
+        <f>IF('Charge 13'!K16=0, "-", 'Charge 13'!K16)</f>
         <v>-</v>
       </c>
-      <c r="E8" s="107" t="str">
-        <f>IF('Charge 12'!K16=0, "-", 'Charge 12'!K16)</f>
-        <v>-</v>
-      </c>
       <c r="F8" s="106" t="str">
-        <f>IF('Charge 12'!N16=0, "-", 'Charge 12'!N16)</f>
+        <f>IF('Charge 13'!N16=0, "-", 'Charge 13'!N16)</f>
         <v>-</v>
       </c>
       <c r="G8" s="106">
@@ -5060,24 +5072,24 @@
       <c r="A9" s="27">
         <v>4</v>
       </c>
-      <c r="B9" s="108" t="str">
-        <f>IF('Charge 12'!B17=0, "-", 'Charge 12'!B17)</f>
+      <c r="B9" s="108">
+        <f>IF('Charge 13'!B17=0, "-", 'Charge 13'!B17)</f>
+        <v>7.2329999999999997</v>
+      </c>
+      <c r="C9" s="107" t="str">
+        <f>IF('Charge 13'!E17=0,"-",'Charge 13'!E17)</f>
         <v>-</v>
       </c>
-      <c r="C9" s="107" t="str">
-        <f>IF('Charge 12'!E17=0,"-",'Charge 12'!E17)</f>
+      <c r="D9" s="107" t="str">
+        <f>IF('Charge 13'!H17=0, "-", 'Charge 13'!H17)</f>
         <v>-</v>
       </c>
-      <c r="D9" s="107" t="str">
-        <f>IF('Charge 12'!H17=0, "-", 'Charge 12'!H17)</f>
+      <c r="E9" s="107" t="str">
+        <f>IF('Charge 13'!K17=0, "-", 'Charge 13'!K17)</f>
         <v>-</v>
       </c>
-      <c r="E9" s="107" t="str">
-        <f>IF('Charge 12'!K17=0, "-", 'Charge 12'!K17)</f>
-        <v>-</v>
-      </c>
       <c r="F9" s="106" t="str">
-        <f>IF('Charge 12'!N17=0, "-", 'Charge 12'!N17)</f>
+        <f>IF('Charge 13'!N17=0, "-", 'Charge 13'!N17)</f>
         <v>-</v>
       </c>
       <c r="G9" s="106">
@@ -5094,23 +5106,23 @@
         <v>5</v>
       </c>
       <c r="B10" s="108" t="str">
-        <f>IF('Charge 12'!B18=0, "-", 'Charge 12'!B18)</f>
+        <f>IF('Charge 13'!B18=0, "-", 'Charge 13'!B18)</f>
         <v>-</v>
       </c>
       <c r="C10" s="107" t="str">
-        <f>IF('Charge 12'!E18=0,"-",'Charge 12'!E18)</f>
+        <f>IF('Charge 13'!E18=0,"-",'Charge 13'!E18)</f>
         <v>-</v>
       </c>
       <c r="D10" s="107" t="str">
-        <f>IF('Charge 12'!H18=0, "-", 'Charge 12'!H18)</f>
+        <f>IF('Charge 13'!H18=0, "-", 'Charge 13'!H18)</f>
         <v>-</v>
       </c>
       <c r="E10" s="107" t="str">
-        <f>IF('Charge 12'!K18=0, "-", 'Charge 12'!K18)</f>
+        <f>IF('Charge 13'!K18=0, "-", 'Charge 13'!K18)</f>
         <v>-</v>
       </c>
       <c r="F10" s="106" t="str">
-        <f>IF('Charge 12'!N18=0, "-", 'Charge 12'!N18)</f>
+        <f>IF('Charge 13'!N18=0, "-", 'Charge 13'!N18)</f>
         <v>-</v>
       </c>
       <c r="G10" s="142">
@@ -5127,28 +5139,28 @@
         <v>6</v>
       </c>
       <c r="B11" s="108" t="str">
-        <f>IF('Charge 12'!B19=0, "-", 'Charge 12'!B19)</f>
+        <f>IF('Charge 13'!B19=0, "-", 'Charge 13'!B19)</f>
         <v>-</v>
       </c>
       <c r="C11" s="107" t="str">
-        <f>IF('Charge 12'!E19=0,"-",'Charge 12'!E19)</f>
+        <f>IF('Charge 13'!E19=0,"-",'Charge 13'!E19)</f>
         <v>-</v>
       </c>
       <c r="D11" s="107" t="str">
-        <f>IF('Charge 12'!H19=0, "-", 'Charge 12'!H19)</f>
+        <f>IF('Charge 13'!H19=0, "-", 'Charge 13'!H19)</f>
         <v>-</v>
       </c>
       <c r="E11" s="107" t="str">
-        <f>IF('Charge 12'!K19=0, "-", 'Charge 12'!K19)</f>
+        <f>IF('Charge 13'!K19=0, "-", 'Charge 13'!K19)</f>
         <v>-</v>
       </c>
       <c r="F11" s="106" t="str">
-        <f>IF('Charge 12'!N19=0, "-", 'Charge 12'!N19)</f>
+        <f>IF('Charge 13'!N19=0, "-", 'Charge 13'!N19)</f>
         <v>-</v>
       </c>
       <c r="G11" s="160">
         <f>COUNTIF(B6:F20, "&lt;&gt;-")</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H11" s="153" t="str">
         <f>G4</f>
@@ -5160,23 +5172,23 @@
         <v>7</v>
       </c>
       <c r="B12" s="108" t="str">
-        <f>IF('Charge 12'!B20=0, "-", 'Charge 12'!B20)</f>
+        <f>IF('Charge 13'!B20=0, "-", 'Charge 13'!B20)</f>
         <v>-</v>
       </c>
       <c r="C12" s="107" t="str">
-        <f>IF('Charge 12'!E20=0,"-",'Charge 12'!E20)</f>
+        <f>IF('Charge 13'!E20=0,"-",'Charge 13'!E20)</f>
         <v>-</v>
       </c>
       <c r="D12" s="107" t="str">
-        <f>IF('Charge 12'!H20=0, "-", 'Charge 12'!H20)</f>
+        <f>IF('Charge 13'!H20=0, "-", 'Charge 13'!H20)</f>
         <v>-</v>
       </c>
       <c r="E12" s="107" t="str">
-        <f>IF('Charge 12'!K20=0, "-", 'Charge 12'!K20)</f>
+        <f>IF('Charge 13'!K20=0, "-", 'Charge 13'!K20)</f>
         <v>-</v>
       </c>
       <c r="F12" s="106" t="str">
-        <f>IF('Charge 12'!N20=0, "-", 'Charge 12'!N20)</f>
+        <f>IF('Charge 13'!N20=0, "-", 'Charge 13'!N20)</f>
         <v>-</v>
       </c>
       <c r="G12" s="106"/>
@@ -5186,23 +5198,23 @@
         <v>8</v>
       </c>
       <c r="B13" s="108" t="str">
-        <f>IF('Charge 12'!B21=0, "-", 'Charge 12'!B21)</f>
+        <f>IF('Charge 13'!B21=0, "-", 'Charge 13'!B21)</f>
         <v>-</v>
       </c>
       <c r="C13" s="107" t="str">
-        <f>IF('Charge 12'!E21=0,"-",'Charge 12'!E21)</f>
+        <f>IF('Charge 13'!E21=0,"-",'Charge 13'!E21)</f>
         <v>-</v>
       </c>
       <c r="D13" s="107" t="str">
-        <f>IF('Charge 12'!H21=0, "-", 'Charge 12'!H21)</f>
+        <f>IF('Charge 13'!H21=0, "-", 'Charge 13'!H21)</f>
         <v>-</v>
       </c>
       <c r="E13" s="107" t="str">
-        <f>IF('Charge 12'!K21=0, "-", 'Charge 12'!K21)</f>
+        <f>IF('Charge 13'!K21=0, "-", 'Charge 13'!K21)</f>
         <v>-</v>
       </c>
       <c r="F13" s="106" t="str">
-        <f>IF('Charge 12'!N21=0, "-", 'Charge 12'!N21)</f>
+        <f>IF('Charge 13'!N21=0, "-", 'Charge 13'!N21)</f>
         <v>-</v>
       </c>
       <c r="G13" s="106"/>
@@ -5212,23 +5224,23 @@
         <v>9</v>
       </c>
       <c r="B14" s="108" t="str">
-        <f>IF('Charge 12'!B22=0, "-", 'Charge 12'!B22)</f>
+        <f>IF('Charge 13'!B22=0, "-", 'Charge 13'!B22)</f>
         <v>-</v>
       </c>
       <c r="C14" s="107" t="str">
-        <f>IF('Charge 12'!E22=0,"-",'Charge 12'!E22)</f>
+        <f>IF('Charge 13'!E22=0,"-",'Charge 13'!E22)</f>
         <v>-</v>
       </c>
       <c r="D14" s="107" t="str">
-        <f>IF('Charge 12'!H22=0, "-", 'Charge 12'!H22)</f>
+        <f>IF('Charge 13'!H22=0, "-", 'Charge 13'!H22)</f>
         <v>-</v>
       </c>
       <c r="E14" s="107" t="str">
-        <f>IF('Charge 12'!K22=0, "-", 'Charge 12'!K22)</f>
+        <f>IF('Charge 13'!K22=0, "-", 'Charge 13'!K22)</f>
         <v>-</v>
       </c>
       <c r="F14" s="106" t="str">
-        <f>IF('Charge 12'!N22=0, "-", 'Charge 12'!N22)</f>
+        <f>IF('Charge 13'!N22=0, "-", 'Charge 13'!N22)</f>
         <v>-</v>
       </c>
       <c r="G14" s="106"/>
@@ -5238,23 +5250,23 @@
         <v>10</v>
       </c>
       <c r="B15" s="108" t="str">
-        <f>IF('Charge 12'!B23=0, "-", 'Charge 12'!B23)</f>
+        <f>IF('Charge 13'!B23=0, "-", 'Charge 13'!B23)</f>
         <v>-</v>
       </c>
       <c r="C15" s="107" t="str">
-        <f>IF('Charge 12'!E23=0,"-",'Charge 12'!E23)</f>
+        <f>IF('Charge 13'!E23=0,"-",'Charge 13'!E23)</f>
         <v>-</v>
       </c>
       <c r="D15" s="107" t="str">
-        <f>IF('Charge 12'!H23=0, "-", 'Charge 12'!H23)</f>
+        <f>IF('Charge 13'!H23=0, "-", 'Charge 13'!H23)</f>
         <v>-</v>
       </c>
       <c r="E15" s="107" t="str">
-        <f>IF('Charge 12'!K23=0, "-", 'Charge 12'!K23)</f>
+        <f>IF('Charge 13'!K23=0, "-", 'Charge 13'!K23)</f>
         <v>-</v>
       </c>
       <c r="F15" s="106" t="str">
-        <f>IF('Charge 12'!N23=0, "-", 'Charge 12'!N23)</f>
+        <f>IF('Charge 13'!N23=0, "-", 'Charge 13'!N23)</f>
         <v>-</v>
       </c>
       <c r="G15" s="106"/>
@@ -5264,23 +5276,23 @@
         <v>11</v>
       </c>
       <c r="B16" s="108" t="str">
-        <f>IF('Charge 12'!B24=0, "-", 'Charge 12'!B24)</f>
+        <f>IF('Charge 13'!B24=0, "-", 'Charge 13'!B24)</f>
         <v>-</v>
       </c>
       <c r="C16" s="107" t="str">
-        <f>IF('Charge 12'!E24=0,"-",'Charge 12'!E24)</f>
+        <f>IF('Charge 13'!E24=0,"-",'Charge 13'!E24)</f>
         <v>-</v>
       </c>
       <c r="D16" s="107" t="str">
-        <f>IF('Charge 12'!H24=0, "-", 'Charge 12'!H24)</f>
+        <f>IF('Charge 13'!H24=0, "-", 'Charge 13'!H24)</f>
         <v>-</v>
       </c>
       <c r="E16" s="107" t="str">
-        <f>IF('Charge 12'!K24=0, "-", 'Charge 12'!K24)</f>
+        <f>IF('Charge 13'!K24=0, "-", 'Charge 13'!K24)</f>
         <v>-</v>
       </c>
       <c r="F16" s="106" t="str">
-        <f>IF('Charge 12'!N24=0, "-", 'Charge 12'!N24)</f>
+        <f>IF('Charge 13'!N24=0, "-", 'Charge 13'!N24)</f>
         <v>-</v>
       </c>
       <c r="G16" s="106"/>
@@ -5290,23 +5302,23 @@
         <v>12</v>
       </c>
       <c r="B17" s="108" t="str">
-        <f>IF('Charge 12'!B25=0, "-", 'Charge 12'!B25)</f>
+        <f>IF('Charge 13'!B25=0, "-", 'Charge 13'!B25)</f>
         <v>-</v>
       </c>
       <c r="C17" s="107" t="str">
-        <f>IF('Charge 12'!E25=0,"-",'Charge 12'!E25)</f>
+        <f>IF('Charge 13'!E25=0,"-",'Charge 13'!E25)</f>
         <v>-</v>
       </c>
       <c r="D17" s="107" t="str">
-        <f>IF('Charge 12'!H25=0, "-", 'Charge 12'!H25)</f>
+        <f>IF('Charge 13'!H25=0, "-", 'Charge 13'!H25)</f>
         <v>-</v>
       </c>
       <c r="E17" s="107" t="str">
-        <f>IF('Charge 12'!K25=0, "-", 'Charge 12'!K25)</f>
+        <f>IF('Charge 13'!K25=0, "-", 'Charge 13'!K25)</f>
         <v>-</v>
       </c>
       <c r="F17" s="106" t="str">
-        <f>IF('Charge 12'!N25=0, "-", 'Charge 12'!N25)</f>
+        <f>IF('Charge 13'!N25=0, "-", 'Charge 13'!N25)</f>
         <v>-</v>
       </c>
       <c r="G17" s="106"/>
@@ -5316,23 +5328,23 @@
         <v>13</v>
       </c>
       <c r="B18" s="108" t="str">
-        <f>IF('Charge 12'!B26=0, "-", 'Charge 12'!B26)</f>
+        <f>IF('Charge 13'!B26=0, "-", 'Charge 13'!B26)</f>
         <v>-</v>
       </c>
       <c r="C18" s="107" t="str">
-        <f>IF('Charge 12'!E26=0,"-",'Charge 12'!E26)</f>
+        <f>IF('Charge 13'!E26=0,"-",'Charge 13'!E26)</f>
         <v>-</v>
       </c>
       <c r="D18" s="107" t="str">
-        <f>IF('Charge 12'!H26=0, "-", 'Charge 12'!H26)</f>
+        <f>IF('Charge 13'!H26=0, "-", 'Charge 13'!H26)</f>
         <v>-</v>
       </c>
       <c r="E18" s="107" t="str">
-        <f>IF('Charge 12'!K26=0, "-", 'Charge 12'!K26)</f>
+        <f>IF('Charge 13'!K26=0, "-", 'Charge 13'!K26)</f>
         <v>-</v>
       </c>
       <c r="F18" s="106" t="str">
-        <f>IF('Charge 12'!N26=0, "-", 'Charge 12'!N26)</f>
+        <f>IF('Charge 13'!N26=0, "-", 'Charge 13'!N26)</f>
         <v>-</v>
       </c>
       <c r="G18" s="106"/>
@@ -5342,23 +5354,23 @@
         <v>14</v>
       </c>
       <c r="B19" s="108" t="str">
-        <f>IF('Charge 12'!B27=0, "-", 'Charge 12'!B27)</f>
+        <f>IF('Charge 13'!B27=0, "-", 'Charge 13'!B27)</f>
         <v>-</v>
       </c>
       <c r="C19" s="107" t="str">
-        <f>IF('Charge 12'!E27=0,"-",'Charge 12'!E27)</f>
+        <f>IF('Charge 13'!E27=0,"-",'Charge 13'!E27)</f>
         <v>-</v>
       </c>
       <c r="D19" s="107" t="str">
-        <f>IF('Charge 12'!H27=0, "-", 'Charge 12'!H27)</f>
+        <f>IF('Charge 13'!H27=0, "-", 'Charge 13'!H27)</f>
         <v>-</v>
       </c>
       <c r="E19" s="107" t="str">
-        <f>IF('Charge 12'!K27=0, "-", 'Charge 12'!K27)</f>
+        <f>IF('Charge 13'!K27=0, "-", 'Charge 13'!K27)</f>
         <v>-</v>
       </c>
       <c r="F19" s="106" t="str">
-        <f>IF('Charge 12'!N27=0, "-", 'Charge 12'!N27)</f>
+        <f>IF('Charge 13'!N27=0, "-", 'Charge 13'!N27)</f>
         <v>-</v>
       </c>
       <c r="G19" s="106"/>
@@ -5368,23 +5380,23 @@
         <v>15</v>
       </c>
       <c r="B20" s="141" t="str">
-        <f>IF('Charge 12'!B28=0, "-", 'Charge 12'!B28)</f>
+        <f>IF('Charge 13'!B28=0, "-", 'Charge 13'!B28)</f>
         <v>-</v>
       </c>
       <c r="C20" s="114" t="str">
-        <f>IF('Charge 12'!E28=0,"-",'Charge 12'!E28)</f>
+        <f>IF('Charge 13'!E28=0,"-",'Charge 13'!E28)</f>
         <v>-</v>
       </c>
       <c r="D20" s="114" t="str">
-        <f>IF('Charge 12'!H28=0, "-", 'Charge 12'!H28)</f>
+        <f>IF('Charge 13'!H28=0, "-", 'Charge 13'!H28)</f>
         <v>-</v>
       </c>
       <c r="E20" s="114" t="str">
-        <f>IF('Charge 12'!K28=0, "-", 'Charge 12'!K28)</f>
+        <f>IF('Charge 13'!K28=0, "-", 'Charge 13'!K28)</f>
         <v>-</v>
       </c>
       <c r="F20" s="142" t="str">
-        <f>IF('Charge 12'!N28=0, "-", 'Charge 12'!N28)</f>
+        <f>IF('Charge 13'!N28=0, "-", 'Charge 13'!N28)</f>
         <v>-</v>
       </c>
       <c r="G20" s="106"/>
@@ -5395,15 +5407,15 @@
       </c>
       <c r="B21" s="77">
         <f>SUM(B6:B20)</f>
-        <v>0</v>
+        <v>24.065000000000001</v>
       </c>
       <c r="C21" s="37">
         <f>SUM(C6:C20)</f>
-        <v>0</v>
+        <v>29.869</v>
       </c>
       <c r="D21" s="69">
         <f>SUM(D6:D20)</f>
-        <v>6.101</v>
+        <v>3.052</v>
       </c>
       <c r="E21" s="69">
         <f>SUM(E6:E20)</f>
@@ -5415,7 +5427,7 @@
       </c>
       <c r="G21" s="144">
         <f>SUM(B21:F21)</f>
-        <v>6.101</v>
+        <v>56.985999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5423,28 +5435,28 @@
         <v>109</v>
       </c>
       <c r="B22" s="145">
-        <f>'Charge 12'!F4</f>
-        <v>48.134</v>
+        <f>'Charge 13'!F4</f>
+        <v>24.061</v>
       </c>
       <c r="C22" s="135">
-        <f>'Charge 12'!F5</f>
-        <v>59.761000000000003</v>
+        <f>'Charge 13'!F5</f>
+        <v>29.873000000000001</v>
       </c>
       <c r="D22" s="135">
-        <f>'Charge 12'!F6</f>
-        <v>6.1050000000000004</v>
+        <f>'Charge 13'!F6</f>
+        <v>3.052</v>
       </c>
       <c r="E22" s="135">
-        <f>'Charge 12'!F7</f>
+        <f>'Charge 13'!F7</f>
         <v>0</v>
       </c>
       <c r="F22" s="139">
-        <f>'Charge 12'!F8</f>
+        <f>'Charge 13'!F8</f>
         <v>0</v>
       </c>
       <c r="G22" s="70">
         <f>SUM(B22:F22)</f>
-        <v>114.00000000000001</v>
+        <v>56.985999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5453,15 +5465,15 @@
       </c>
       <c r="B23" s="146">
         <f>B21-B22</f>
-        <v>-48.134</v>
+        <v>4.0000000000013358E-3</v>
       </c>
       <c r="C23" s="140">
         <f t="shared" ref="C23:G23" si="0">C21-C22</f>
-        <v>-59.761000000000003</v>
+        <v>-4.0000000000013358E-3</v>
       </c>
       <c r="D23" s="140">
         <f t="shared" si="0"/>
-        <v>-4.0000000000004476E-3</v>
+        <v>0</v>
       </c>
       <c r="E23" s="140">
         <f t="shared" si="0"/>
@@ -5473,7 +5485,7 @@
       </c>
       <c r="G23" s="113">
         <f t="shared" si="0"/>
-        <v>-107.89900000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -5499,7 +5511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5569,7 +5581,7 @@
       </c>
       <c r="I3" s="62" t="str">
         <f>Q4 &amp; ROUND(N4,3)*100 &amp; IF(N5=0, "", Q5 &amp; ROUND(N5,3)*100) &amp; IF(N6=0, "", Q6 &amp; ROUND(N6,3)*100) &amp; IF(N7=0, "", Q7 &amp; ROUND(N7,3)*100) &amp; IF(N8=0, "", Q8 &amp; ROUND(N8,3)*100)</f>
-        <v>Mg0Ca100</v>
+        <v>Mg65Zn30Ca5</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="s">
@@ -5662,11 +5674,11 @@
       </c>
       <c r="F4" s="69">
         <f>IF($F$9=0, ROUND($F$10*E4, 3), ROUND(E4*$F$9, 3))</f>
-        <v>48.134</v>
+        <v>24.061</v>
       </c>
       <c r="G4" s="70">
         <f>IFERROR(F4/U4, 0)</f>
-        <v>27.69505178365938</v>
+        <v>13.844073647871117</v>
       </c>
       <c r="I4" s="71" t="str">
         <f>$Q$4</f>
@@ -5675,19 +5687,19 @@
       <c r="J4" s="26"/>
       <c r="K4" s="72">
         <f>B29</f>
-        <v>0</v>
+        <v>24.065000000000001</v>
       </c>
       <c r="L4" s="73">
         <f>K4/$K$9</f>
-        <v>0</v>
+        <v>0.42229670445372552</v>
       </c>
       <c r="M4" s="23">
         <f>IFERROR(L4/T4, 0)</f>
-        <v>0</v>
+        <v>1.7374890123584674E-2</v>
       </c>
       <c r="N4" s="115">
         <f>M4/$M$9</f>
-        <v>0</v>
+        <v>0.65006602602116492</v>
       </c>
       <c r="P4" s="15">
         <v>1</v>
@@ -5759,11 +5771,11 @@
       </c>
       <c r="F5" s="69">
         <f t="shared" ref="F5:F8" si="0">IF($F$9=0, ROUND($F$10*E5, 3), ROUND(E5*$F$9, 3))</f>
-        <v>59.761000000000003</v>
+        <v>29.873000000000001</v>
       </c>
       <c r="G5" s="70">
         <f>IFERROR(F5/U5, 0)</f>
-        <v>8.3698879551820742</v>
+        <v>4.1838935574229694</v>
       </c>
       <c r="I5" s="71" t="str">
         <f>$Q$5</f>
@@ -5772,19 +5784,19 @@
       <c r="J5" s="27"/>
       <c r="K5" s="75">
         <f>E29</f>
-        <v>0</v>
+        <v>29.869</v>
       </c>
       <c r="L5" s="76">
         <f>K5/$K$9</f>
-        <v>0</v>
+        <v>0.52414628154283516</v>
       </c>
       <c r="M5" s="24">
         <f>IFERROR(L5/T5, 0)</f>
-        <v>0</v>
+        <v>8.0166755612069845E-3</v>
       </c>
       <c r="N5" s="116">
         <f>M5/$M$9</f>
-        <v>0</v>
+        <v>0.29993677006917618</v>
       </c>
       <c r="P5" s="15">
         <v>2</v>
@@ -5856,11 +5868,11 @@
       </c>
       <c r="F6" s="69">
         <f t="shared" si="0"/>
-        <v>6.1050000000000004</v>
+        <v>3.052</v>
       </c>
       <c r="G6" s="70">
         <f>IFERROR(F6/U6, 0)</f>
-        <v>3.9387096774193551</v>
+        <v>1.9690322580645161</v>
       </c>
       <c r="I6" s="71" t="str">
         <f>$Q$6</f>
@@ -5869,19 +5881,19 @@
       <c r="J6" s="27"/>
       <c r="K6" s="77">
         <f>H29</f>
-        <v>6.101</v>
+        <v>3.052</v>
       </c>
       <c r="L6" s="76">
         <f>K6/$K$9</f>
-        <v>1</v>
+        <v>5.3557014003439443E-2</v>
       </c>
       <c r="M6" s="24">
         <f>IFERROR(L6/T6, 0)</f>
-        <v>2.4951344877488894E-2</v>
+        <v>1.3363195270083197E-3</v>
       </c>
       <c r="N6" s="116">
         <f>M6/$M$9</f>
-        <v>1</v>
+        <v>4.999720390965888E-2</v>
       </c>
       <c r="P6" s="15">
         <v>3</v>
@@ -6149,7 +6161,7 @@
       </c>
       <c r="G9" s="144">
         <f>SUM(G4:G8)</f>
-        <v>40.003649416260807</v>
+        <v>19.996999463358602</v>
       </c>
       <c r="I9" s="82"/>
       <c r="J9" s="79" t="s">
@@ -6157,7 +6169,7 @@
       </c>
       <c r="K9" s="117">
         <f>SUM(K4:K8)</f>
-        <v>6.101</v>
+        <v>56.985999999999997</v>
       </c>
       <c r="L9" s="83">
         <f>SUM(L4:L8)</f>
@@ -6165,7 +6177,7 @@
       </c>
       <c r="M9" s="118">
         <f>SUM(M4:M8)</f>
-        <v>2.4951344877488894E-2</v>
+        <v>2.672788521179998E-2</v>
       </c>
       <c r="N9" s="84">
         <f>SUM(N4:N8)</f>
@@ -6211,10 +6223,10 @@
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F10" s="158">
         <f>G10*U9</f>
-        <v>114</v>
+        <v>56.985750000000003</v>
       </c>
       <c r="G10" s="9">
-        <v>40</v>
+        <v>19.995000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="26.25" x14ac:dyDescent="0.4">
@@ -6320,7 +6332,7 @@
       </c>
       <c r="B14" s="106">
         <f>A!C2</f>
-        <v>0</v>
+        <v>5.0609999999999999</v>
       </c>
       <c r="C14" s="107"/>
       <c r="D14" s="126">
@@ -6328,7 +6340,7 @@
       </c>
       <c r="E14" s="106">
         <f>B!C2</f>
-        <v>0</v>
+        <v>10.72</v>
       </c>
       <c r="F14" s="107"/>
       <c r="G14" s="126">
@@ -6336,7 +6348,7 @@
       </c>
       <c r="H14" s="106">
         <f>'C'!C2</f>
-        <v>6.101</v>
+        <v>3.052</v>
       </c>
       <c r="I14" s="107"/>
       <c r="J14" s="126">
@@ -6373,7 +6385,7 @@
       </c>
       <c r="B15" s="106">
         <f>A!C3</f>
-        <v>0</v>
+        <v>5.6879999999999997</v>
       </c>
       <c r="C15" s="107"/>
       <c r="D15" s="126">
@@ -6381,7 +6393,7 @@
       </c>
       <c r="E15" s="106">
         <f>B!C3</f>
-        <v>0</v>
+        <v>19.149000000000001</v>
       </c>
       <c r="F15" s="107"/>
       <c r="G15" s="126">
@@ -6426,7 +6438,7 @@
       </c>
       <c r="B16" s="106">
         <f>A!C4</f>
-        <v>0</v>
+        <v>6.0830000000000002</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="126">
@@ -6479,7 +6491,7 @@
       </c>
       <c r="B17" s="106">
         <f>A!C5</f>
-        <v>0</v>
+        <v>7.2329999999999997</v>
       </c>
       <c r="C17" s="107"/>
       <c r="D17" s="126">
@@ -6625,7 +6637,9 @@
         <v>99</v>
       </c>
       <c r="Q19" s="8"/>
-      <c r="R19" s="10"/>
+      <c r="R19" s="10" t="s">
+        <v>194</v>
+      </c>
       <c r="S19" s="7"/>
       <c r="T19" s="8"/>
       <c r="V19"/>
@@ -6676,7 +6690,9 @@
         <v>100</v>
       </c>
       <c r="Q20" s="8"/>
-      <c r="R20" s="10"/>
+      <c r="R20" s="10" t="s">
+        <v>195</v>
+      </c>
       <c r="S20" s="7"/>
       <c r="T20" s="8"/>
       <c r="V20"/>
@@ -7034,7 +7050,7 @@
       </c>
       <c r="B29" s="110">
         <f>SUM(B14:B28)</f>
-        <v>0</v>
+        <v>24.065000000000001</v>
       </c>
       <c r="C29" s="107"/>
       <c r="D29" s="109" t="s">
@@ -7042,7 +7058,7 @@
       </c>
       <c r="E29" s="111">
         <f>SUM(E14:E28)</f>
-        <v>0</v>
+        <v>29.869</v>
       </c>
       <c r="F29" s="107"/>
       <c r="G29" s="109" t="s">
@@ -7050,7 +7066,7 @@
       </c>
       <c r="H29" s="110">
         <f>SUM(H14:H28)</f>
-        <v>6.101</v>
+        <v>3.052</v>
       </c>
       <c r="I29" s="107"/>
       <c r="J29" s="109" t="s">
@@ -7075,7 +7091,7 @@
       </c>
       <c r="B30" s="113">
         <f>B29-$F$4</f>
-        <v>-48.134</v>
+        <v>4.0000000000013358E-3</v>
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="112" t="s">
@@ -7083,7 +7099,7 @@
       </c>
       <c r="E30" s="113">
         <f>E29-$F$5</f>
-        <v>-59.761000000000003</v>
+        <v>-4.0000000000013358E-3</v>
       </c>
       <c r="F30" s="114"/>
       <c r="G30" s="112" t="s">
@@ -7091,7 +7107,7 @@
       </c>
       <c r="H30" s="113">
         <f>H29-$F$6</f>
-        <v>-4.0000000000004476E-3</v>
+        <v>0</v>
       </c>
       <c r="I30" s="114"/>
       <c r="J30" s="112" t="s">
@@ -7188,7 +7204,9 @@
       <c r="J34" s="43"/>
       <c r="K34" s="43"/>
       <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
+      <c r="M34" s="43" t="s">
+        <v>196</v>
+      </c>
       <c r="N34" s="43"/>
       <c r="O34" s="43"/>
       <c r="P34" s="43"/>
@@ -7220,7 +7238,9 @@
       <c r="J35" s="43"/>
       <c r="K35" s="49"/>
       <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
+      <c r="M35" s="43" t="s">
+        <v>197</v>
+      </c>
       <c r="N35" s="43"/>
       <c r="O35" s="43"/>
       <c r="P35" s="43"/>
@@ -8487,7 +8507,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -8525,22 +8545,22 @@
         <v>5.0609999999999999</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <v>5.0609999999999999</v>
       </c>
       <c r="D2" s="1">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>24.065000000000001</v>
       </c>
       <c r="E2" s="127" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="129">
-        <f>'Charge 12'!F4</f>
-        <v>48.134</v>
+        <f>'Charge 13'!F4</f>
+        <v>24.061</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8548,11 +8568,11 @@
         <v>5.6879999999999997</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.6879999999999997</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="127" t="s">
@@ -8560,7 +8580,7 @@
       </c>
       <c r="F3" s="129">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>24.065000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -8568,11 +8588,11 @@
         <v>6.0830000000000002</v>
       </c>
       <c r="B4" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6.0830000000000002</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="127" t="s">
@@ -8580,43 +8600,43 @@
       </c>
       <c r="F4" s="129">
         <f>F3-F2</f>
-        <v>-48.134</v>
+        <v>4.0000000000013358E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="166">
-        <v>6.2190000000000003</v>
+        <v>7.2329999999999997</v>
       </c>
       <c r="B5" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7.2329999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="166">
-        <v>6.7640000000000002</v>
+        <v>6.2190000000000003</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6" s="167"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="166">
-        <v>7.2329999999999997</v>
+        <v>6.7640000000000002</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8628,7 +8648,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8640,7 +8660,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8652,7 +8672,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8664,7 +8684,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8674,7 +8694,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8684,7 +8704,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8694,7 +8714,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8704,7 +8724,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8714,7 +8734,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8724,7 +8744,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8734,7 +8754,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8744,7 +8764,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8754,7 +8774,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8764,7 +8784,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8774,7 +8794,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8784,7 +8804,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8794,7 +8814,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8804,7 +8824,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8814,7 +8834,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8824,7 +8844,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8834,7 +8854,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8844,7 +8864,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8854,7 +8874,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8864,7 +8884,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8874,7 +8894,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8884,7 +8904,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -8894,7 +8914,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -8904,7 +8924,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8914,7 +8934,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8924,7 +8944,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8934,7 +8954,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8944,7 +8964,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8954,7 +8974,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8964,7 +8984,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8974,7 +8994,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8984,7 +9004,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8994,7 +9014,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9004,7 +9024,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9014,7 +9034,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9024,7 +9044,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9034,7 +9054,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9044,7 +9064,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9054,7 +9074,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9064,14 +9084,14 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9088,7 +9108,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -9123,55 +9143,55 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>9.782</v>
+        <v>10.72</v>
       </c>
       <c r="B2" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f>IF(A2=0, 0, A2*B2)</f>
-        <v>0</v>
+        <f t="shared" ref="C2:C33" si="0">IF(A2=0, 0, A2*B2)</f>
+        <v>10.72</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>29.869</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
-        <f>'Charge 12'!F5</f>
-        <v>59.761000000000003</v>
+        <f>'Charge 13'!F5</f>
+        <v>29.873000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="125">
-        <v>10.72</v>
+        <v>19.149000000000001</v>
       </c>
       <c r="B3" s="125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f>IF(A3=0, 0, A3*B3)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>19.149000000000001</v>
       </c>
       <c r="E3" s="50" t="s">
         <v>105</v>
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>0</v>
+        <v>29.869</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="125">
-        <v>12.731</v>
+        <v>9.782</v>
       </c>
       <c r="B4" s="125">
         <v>0</v>
       </c>
       <c r="C4">
-        <f>IF(A4=0, 0, A4*B4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="50" t="s">
@@ -9179,66 +9199,66 @@
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-59.761000000000003</v>
+        <v>-4.0000000000013358E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="125">
-        <v>12.920999999999999</v>
+        <v>12.731</v>
       </c>
       <c r="B5" s="125">
         <v>0</v>
       </c>
       <c r="C5">
-        <f>IF(A5=0, 0, A5*B5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="125">
-        <v>14.746</v>
+        <v>12.920999999999999</v>
       </c>
       <c r="B6" s="125">
         <v>0</v>
       </c>
       <c r="C6">
-        <f>IF(A6=0, 0, A6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="125">
-        <v>16.824999999999999</v>
+        <v>14.746</v>
       </c>
       <c r="B7" s="125">
         <v>0</v>
       </c>
       <c r="C7">
-        <f>IF(A7=0, 0, A7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="125">
-        <v>17.745999999999999</v>
+        <v>16.824999999999999</v>
       </c>
       <c r="B8" s="125">
         <v>0</v>
       </c>
       <c r="C8">
-        <f>IF(A8=0, 0, A8*B8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="125">
-        <v>19.149000000000001</v>
+        <v>17.745999999999999</v>
       </c>
       <c r="B9" s="125">
         <v>0</v>
       </c>
       <c r="C9">
-        <f>IF(A9=0, 0, A9*B9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9250,7 +9270,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(A10=0, 0, A10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9262,7 +9282,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <f>IF(A11=0, 0, A11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9274,7 +9294,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <f>IF(A12=0, 0, A12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9286,7 +9306,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <f>IF(A13=0, 0, A13*B13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9298,7 +9318,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>IF(A14=0, 0, A14*B14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9310,7 +9330,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>IF(A15=0, 0, A15*B15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9320,7 +9340,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f>IF(A16=0, 0, A16*B16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9330,7 +9350,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f>IF(A17=0, 0, A17*B17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9340,7 +9360,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>IF(A18=0, 0, A18*B18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9350,7 +9370,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>IF(A19=0, 0, A19*B19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9360,7 +9380,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <f>IF(A20=0, 0, A20*B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9370,7 +9390,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <f>IF(A21=0, 0, A21*B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9380,7 +9400,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <f>IF(A22=0, 0, A22*B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9390,7 +9410,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <f>IF(A23=0, 0, A23*B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9400,7 +9420,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <f>IF(A24=0, 0, A24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9410,7 +9430,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <f>IF(A25=0, 0, A25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9420,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <f>IF(A26=0, 0, A26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9430,7 +9450,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f>IF(A27=0, 0, A27*B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9440,7 +9460,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <f>IF(A28=0, 0, A28*B28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9450,7 +9470,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <f>IF(A29=0, 0, A29*B29)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9460,7 +9480,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <f>IF(A30=0, 0, A30*B30)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9470,7 +9490,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <f>IF(A31=0, 0, A31*B31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9480,7 +9500,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <f>IF(A32=0, 0, A32*B32)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9490,7 +9510,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f>IF(A33=0, 0, A33*B33)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -9500,7 +9520,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <f>IF(A34=0, 0, A34*B34)</f>
+        <f t="shared" ref="C34:C51" si="1">IF(A34=0, 0, A34*B34)</f>
         <v>0</v>
       </c>
     </row>
@@ -9510,7 +9530,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <f>IF(A35=0, 0, A35*B35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9520,7 +9540,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <f>IF(A36=0, 0, A36*B36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9530,7 +9550,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <f>IF(A37=0, 0, A37*B37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9540,7 +9560,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <f>IF(A38=0, 0, A38*B38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9550,7 +9570,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <f>IF(A39=0, 0, A39*B39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9560,7 +9580,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <f>IF(A40=0, 0, A40*B40)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9570,7 +9590,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <f>IF(A41=0, 0, A41*B41)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9580,7 +9600,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f>IF(A42=0, 0, A42*B42)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9590,7 +9610,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <f>IF(A43=0, 0, A43*B43)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9600,7 +9620,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <f>IF(A44=0, 0, A44*B44)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9610,7 +9630,7 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <f>IF(A45=0, 0, A45*B45)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9620,7 +9640,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <f>IF(A46=0, 0, A46*B46)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9630,7 +9650,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <f>IF(A47=0, 0, A47*B47)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9640,7 +9660,7 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <f>IF(A48=0, 0, A48*B48)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9650,7 +9670,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <f>IF(A49=0, 0, A49*B49)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9660,7 +9680,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <f>IF(A50=0, 0, A50*B50)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -9670,14 +9690,14 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <f>IF(A51=0, 0, A51*B51)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1">
     <sortState ref="A2:C51">
-      <sortCondition ref="A1"/>
+      <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9729,25 +9749,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="125">
-        <v>6.101</v>
+        <v>3.052</v>
       </c>
       <c r="B2" s="125">
         <v>1</v>
       </c>
       <c r="C2">
         <f>IF(A2=0, 0, A2*B2)</f>
-        <v>6.101</v>
+        <v>3.052</v>
       </c>
       <c r="D2">
         <f>SUM(C:C)</f>
-        <v>6.101</v>
+        <v>3.052</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>109</v>
       </c>
       <c r="F2" s="51">
-        <f>'Charge 12'!F6</f>
-        <v>6.1050000000000004</v>
+        <f>'Charge 13'!F6</f>
+        <v>3.052</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9764,7 +9784,7 @@
       </c>
       <c r="F3" s="51">
         <f>SUM(C:C)</f>
-        <v>6.101</v>
+        <v>3.052</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9781,7 +9801,7 @@
       </c>
       <c r="F4" s="51">
         <f>F3-F2</f>
-        <v>-4.0000000000004476E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -10324,7 +10344,7 @@
         <v>109</v>
       </c>
       <c r="F2" s="51">
-        <f>'Charge 12'!F7</f>
+        <f>'Charge 13'!F7</f>
         <v>0</v>
       </c>
     </row>
@@ -10902,7 +10922,7 @@
         <v>109</v>
       </c>
       <c r="F2" s="51">
-        <f>'Charge 12'!F8</f>
+        <f>'Charge 13'!F8</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>